<commit_message>
461 hamming distance weaknesses and time complexity
</commit_message>
<xml_diff>
--- a/leetcode.xlsx
+++ b/leetcode.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umbc-my.sharepoint.com/personal/venkati1_umbc_edu/Documents/Desktop/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{A8A03DBA-34ED-4B50-8814-B16395810788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F283800-F4EA-4D45-8D11-F806B801A72F}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{A8A03DBA-34ED-4B50-8814-B16395810788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC69A6DB-7E08-4709-8D8D-CB6264CCCFD7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9E5C2B37-1DB0-4385-BC19-116E7A02A46A}"/>
+    <workbookView minimized="1" xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8880" xr2:uid="{9E5C2B37-1DB0-4385-BC19-116E7A02A46A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="337">
   <si>
     <t>S.No</t>
   </si>
@@ -1011,9 +1011,6 @@
     <t>2130. Maximum Twin Sum of a Linked List</t>
   </si>
   <si>
-    <t>category</t>
-  </si>
-  <si>
     <t>linked list</t>
   </si>
   <si>
@@ -1023,9 +1020,6 @@
     <t>Easy</t>
   </si>
   <si>
-    <t>patterns</t>
-  </si>
-  <si>
     <t>142. Linked List Cycle II , 202. Happy Number</t>
   </si>
   <si>
@@ -1033,13 +1027,78 @@
   </si>
   <si>
     <t>141. Linked List Cycle</t>
+  </si>
+  <si>
+    <r>
+      <t>190. Reverse Bits</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">,  </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">231. Power of Two </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>338. Counting Bits</t>
+    </r>
+  </si>
+  <si>
+    <t>binary search</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of 1 bits </t>
+  </si>
+  <si>
+    <t>Patterns</t>
+  </si>
+  <si>
+    <t>The idea is to remove the rightmost one from n's binary. Which can be achieved by Subtracting 1 from n and perform bitwise operation between n and n-1.</t>
+  </si>
+  <si>
+    <t>Approach</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1099,6 +1158,13 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Aptos Narrow"/>
@@ -1268,28 +1334,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1625,20 +1697,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B1BA3D-5506-4E43-B23E-35E57A8317A2}">
-  <dimension ref="B2:H7"/>
+  <dimension ref="B2:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="71" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="129.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="58.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1646,10 +1720,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>324</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -1657,8 +1731,11 @@
       <c r="H2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
@@ -1669,13 +1746,13 @@
         <v>216</v>
       </c>
       <c r="G3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
@@ -1683,19 +1760,19 @@
         <v>234</v>
       </c>
       <c r="E4" t="s">
+        <v>324</v>
+      </c>
+      <c r="F4" t="s">
         <v>325</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>326</v>
-      </c>
-      <c r="G4" t="s">
-        <v>327</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3</v>
       </c>
@@ -1703,28 +1780,45 @@
         <v>141</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G5" t="s">
+        <v>326</v>
+      </c>
+      <c r="H5" t="s">
         <v>327</v>
       </c>
-      <c r="H5" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="H6" s="18"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>191</v>
+      </c>
+      <c r="D6" t="s">
+        <v>333</v>
+      </c>
+      <c r="E6" t="s">
+        <v>332</v>
+      </c>
+      <c r="F6" t="s">
+        <v>331</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
20 valid Paranthesis solution
</commit_message>
<xml_diff>
--- a/leetcode.xlsx
+++ b/leetcode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umbc-my.sharepoint.com/personal/venkati1_umbc_edu/Documents/Desktop/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="8_{A8A03DBA-34ED-4B50-8814-B16395810788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84609FFF-9C4F-4293-BB6E-18F06937E63F}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="8_{A8A03DBA-34ED-4B50-8814-B16395810788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD64A965-5B10-4FAB-814C-626B07EDE1FF}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8880" xr2:uid="{9E5C2B37-1DB0-4385-BC19-116E7A02A46A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9E5C2B37-1DB0-4385-BC19-116E7A02A46A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="342">
   <si>
     <t>S.No</t>
   </si>
@@ -1098,6 +1098,15 @@
   </si>
   <si>
     <t>Hamming distance</t>
+  </si>
+  <si>
+    <t>22. Generate Parentheses, 32. Longest Valid Parentheses, 301. Remove Invalid Parentheses</t>
+  </si>
+  <si>
+    <t>Valid Paranthesis</t>
+  </si>
+  <si>
+    <t>logic and concept and clarity</t>
   </si>
 </sst>
 </file>
@@ -1703,17 +1712,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B1BA3D-5506-4E43-B23E-35E57A8317A2}">
-  <dimension ref="B2:I7"/>
+  <dimension ref="B2:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="71" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="129.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="58.21875" customWidth="1"/>
   </cols>
@@ -1817,6 +1826,9 @@
       <c r="F6" t="s">
         <v>337</v>
       </c>
+      <c r="G6" t="s">
+        <v>326</v>
+      </c>
       <c r="H6" s="19" t="s">
         <v>330</v>
       </c>
@@ -1840,8 +1852,31 @@
       <c r="F7" t="s">
         <v>337</v>
       </c>
+      <c r="G7" t="s">
+        <v>326</v>
+      </c>
       <c r="H7" s="18" t="s">
         <v>336</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>340</v>
+      </c>
+      <c r="E8" t="s">
+        <v>341</v>
+      </c>
+      <c r="G8" t="s">
+        <v>326</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>